<commit_message>
CSV for the seasonal data
</commit_message>
<xml_diff>
--- a/USA.xlsx
+++ b/USA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark Naguib\Desktop\Uni 3rd year\SQL\pizza\DeltaHacks5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brlno\Documents\DeltaHacks5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55570EE-042F-4B55-90B2-FDA6DA29C2D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CD143D-CDE3-45F9-B7AF-F276D160EDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{4E1598AD-BBC5-43CE-B8CB-97F15447FFC7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{4E1598AD-BBC5-43CE-B8CB-97F15447FFC7}"/>
   </bookViews>
   <sheets>
     <sheet name="Early January" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -813,43 +815,43 @@
       <selection sqref="A1:CP7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="12" width="13.26171875" customWidth="1"/>
-    <col min="14" max="14" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.83984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.734375" customWidth="1"/>
-    <col min="23" max="23" width="10.3671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.20703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="12.20703125" customWidth="1"/>
-    <col min="33" max="33" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.41796875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.578125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="10.1015625" customWidth="1"/>
-    <col min="41" max="41" width="13.62890625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="10.1015625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="9.1015625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="9.1015625" customWidth="1"/>
-    <col min="49" max="49" width="9.47265625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="51" max="53" width="13.3671875" customWidth="1"/>
-    <col min="58" max="58" width="9.3671875" bestFit="1" customWidth="1"/>
-    <col min="59" max="61" width="9.3671875" customWidth="1"/>
-    <col min="64" max="64" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="10.41796875" customWidth="1"/>
-    <col min="77" max="77" width="9.05078125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="10.62890625" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="12.9453125" bestFit="1" customWidth="1"/>
-    <col min="85" max="85" width="12.9453125" customWidth="1"/>
-    <col min="91" max="91" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="92" max="92" width="12.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="12" width="13.21875" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.77734375" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="12.21875" customWidth="1"/>
+    <col min="33" max="33" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.109375" customWidth="1"/>
+    <col min="41" max="41" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="9.109375" customWidth="1"/>
+    <col min="49" max="49" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="51" max="53" width="13.33203125" customWidth="1"/>
+    <col min="58" max="58" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="59" max="61" width="9.33203125" customWidth="1"/>
+    <col min="64" max="64" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.44140625" customWidth="1"/>
+    <col min="77" max="77" width="9" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="13" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="13" customWidth="1"/>
+    <col min="91" max="91" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="92" max="92" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1258,7 +1260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1379,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1576,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2126,7 +2128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:94" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2282,7 +2284,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2294,7 +2296,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2306,7 +2308,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2318,7 +2320,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2330,7 +2332,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2342,7 +2344,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2354,7 +2356,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2366,7 +2368,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2378,7 +2380,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2390,7 +2392,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2401,37 +2403,37 @@
   <dimension ref="A1:DX7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="DH1" workbookViewId="0">
-      <selection activeCell="DY8" sqref="DY8"/>
+      <selection activeCell="DW3" sqref="DW3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="13.15625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.15625" customWidth="1"/>
-    <col min="15" max="15" width="11.7890625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.7890625" customWidth="1"/>
-    <col min="18" max="18" width="13.47265625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.47265625" customWidth="1"/>
-    <col min="21" max="21" width="9.7890625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.734375" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.3671875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.20703125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.5234375" bestFit="1" customWidth="1"/>
-    <col min="38" max="39" width="9.5234375" customWidth="1"/>
+    <col min="11" max="11" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.77734375" customWidth="1"/>
+    <col min="18" max="18" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" customWidth="1"/>
+    <col min="21" max="21" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="9.5546875" customWidth="1"/>
     <col min="46" max="46" width="11" bestFit="1" customWidth="1"/>
     <col min="47" max="47" width="11" customWidth="1"/>
-    <col min="48" max="48" width="11.1015625" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="13.62890625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.578125" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.3671875" bestFit="1" customWidth="1"/>
-    <col min="89" max="89" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="10.41796875" customWidth="1"/>
-    <col min="92" max="92" width="12.05078125" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="13.41796875" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="10.62890625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="10.44140625" customWidth="1"/>
+    <col min="92" max="92" width="12" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2817,7 +2819,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -3037,6 +3039,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DI2" t="b">
+        <v>0</v>
+      </c>
       <c r="DJ2" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3049,6 +3054,12 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DM2" t="b">
+        <v>0</v>
+      </c>
+      <c r="DN2" t="b">
+        <v>0</v>
+      </c>
       <c r="DO2" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3065,10 +3076,19 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DS2" t="b">
+        <v>0</v>
+      </c>
+      <c r="DT2" t="b">
+        <v>0</v>
+      </c>
       <c r="DU2" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DV2" t="b">
+        <v>0</v>
+      </c>
       <c r="DW2" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3078,7 +3098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -3298,6 +3318,18 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DL3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DM3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DN3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DO3" t="b">
+        <v>0</v>
+      </c>
       <c r="DP3" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3314,12 +3346,24 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DT3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DU3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DV3" t="b">
+        <v>0</v>
+      </c>
+      <c r="DW3" t="b">
+        <v>0</v>
+      </c>
       <c r="DX3" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -3459,6 +3503,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DI4" t="b">
+        <v>0</v>
+      </c>
       <c r="DJ4" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3467,6 +3514,18 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DL4" t="b">
+        <v>0</v>
+      </c>
+      <c r="DM4" t="b">
+        <v>0</v>
+      </c>
+      <c r="DN4" t="b">
+        <v>0</v>
+      </c>
+      <c r="DO4" t="b">
+        <v>0</v>
+      </c>
       <c r="DP4" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3479,16 +3538,28 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DS4" t="b">
+        <v>0</v>
+      </c>
+      <c r="DT4" t="b">
+        <v>0</v>
+      </c>
       <c r="DU4" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DV4" t="b">
+        <v>0</v>
+      </c>
+      <c r="DW4" t="b">
+        <v>0</v>
+      </c>
       <c r="DX4" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -3832,10 +3903,19 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DK5" t="b">
+        <v>0</v>
+      </c>
       <c r="DL5" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DM5" t="b">
+        <v>0</v>
+      </c>
+      <c r="DN5" t="b">
+        <v>0</v>
+      </c>
       <c r="DO5" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3852,6 +3932,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DS5" t="b">
+        <v>0</v>
+      </c>
       <c r="DT5" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -3860,12 +3943,18 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DV5" t="b">
+        <v>0</v>
+      </c>
+      <c r="DW5" t="b">
+        <v>0</v>
+      </c>
       <c r="DX5" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -4234,7 +4323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:128" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -4550,6 +4639,9 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
+      <c r="DK7" t="b">
+        <v>0</v>
+      </c>
       <c r="DL7" t="b">
         <f>TRUE</f>
         <v>1</v>
@@ -4577,6 +4669,9 @@
       <c r="DR7" t="b">
         <f>TRUE</f>
         <v>1</v>
+      </c>
+      <c r="DS7" t="b">
+        <v>0</v>
       </c>
       <c r="DT7" t="b">
         <f>TRUE</f>
@@ -4610,7 +4705,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4622,7 +4717,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4634,7 +4729,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4646,7 +4741,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4658,7 +4753,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4670,7 +4765,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4682,7 +4777,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4694,7 +4789,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4706,7 +4801,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4718,7 +4813,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4730,7 +4825,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4742,7 +4837,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>